<commit_message>
Make input more consistent
</commit_message>
<xml_diff>
--- a/test/_Input/arguments_2E.xlsx
+++ b/test/_Input/arguments_2E.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\a PSI\Data\Data analysis\XPEEM_toolkit\test\_Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319EA85E-1F00-4875-AE31-75BAE713E17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820D0EAF-AA44-46B6-A135-A52F227D636D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2569,7 +2569,7 @@
   <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>